<commit_message>
Update isMirror = Falso
</commit_message>
<xml_diff>
--- a/resources/annotated_java.xlsx
+++ b/resources/annotated_java.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4441" uniqueCount="1662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4440" uniqueCount="1662">
   <si>
     <t>owner</t>
   </si>
@@ -6379,8 +6379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W633"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:W1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6563,8 +6563,8 @@
       <c r="D3" s="5">
         <v>43700.501516203702</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>70</v>
+      <c r="E3" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="F3" s="6">
         <v>95935</v>

</xml_diff>

<commit_message>
Count xml file in DBcode, Update DBCode and Dependencies, remove projects from corpus
</commit_message>
<xml_diff>
--- a/resources/annotated_java.xlsx
+++ b/resources/annotated_java.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3809" uniqueCount="1660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3816" uniqueCount="1664">
   <si>
     <t>owner</t>
   </si>
@@ -5022,6 +5022,18 @@
   </si>
   <si>
     <t>ZXing ("Zebra Crossing") barcode scanning library for Java, Android</t>
+  </si>
+  <si>
+    <t>Deprecated</t>
+  </si>
+  <si>
+    <t>Archived</t>
+  </si>
+  <si>
+    <t>Moved</t>
+  </si>
+  <si>
+    <t>Inactive</t>
   </si>
 </sst>
 </file>
@@ -5031,7 +5043,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5054,6 +5066,11 @@
       <u/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -5135,7 +5152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -5210,6 +5227,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6376,8 +6394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W633"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A577" workbookViewId="0">
+      <selection activeCell="U626" sqref="U626"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20117,7 +20135,9 @@
       <c r="T196" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="U196" s="12"/>
+      <c r="U196" s="12" t="s">
+        <v>1660</v>
+      </c>
       <c r="V196" s="12"/>
       <c r="W196" s="10" t="s">
         <v>544</v>
@@ -36629,7 +36649,9 @@
       <c r="T432" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="U432" s="20"/>
+      <c r="U432" s="20" t="s">
+        <v>1661</v>
+      </c>
       <c r="V432" s="20" t="s">
         <v>29</v>
       </c>
@@ -36699,7 +36721,9 @@
       <c r="T433" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="U433" s="20"/>
+      <c r="U433" s="20" t="s">
+        <v>1661</v>
+      </c>
       <c r="V433" s="20" t="s">
         <v>29</v>
       </c>
@@ -42787,7 +42811,9 @@
       <c r="T520" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="U520" s="6"/>
+      <c r="U520" s="6" t="s">
+        <v>1662</v>
+      </c>
       <c r="V520" s="15" t="s">
         <v>66</v>
       </c>
@@ -43907,7 +43933,9 @@
       <c r="T536" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="U536" s="6"/>
+      <c r="U536" s="6" t="s">
+        <v>1663</v>
+      </c>
       <c r="V536" s="15" t="s">
         <v>478</v>
       </c>
@@ -48667,7 +48695,9 @@
       <c r="T604" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="U604" s="6"/>
+      <c r="U604" s="26" t="s">
+        <v>1660</v>
+      </c>
       <c r="V604" s="6" t="s">
         <v>164</v>
       </c>
@@ -50417,7 +50447,9 @@
       <c r="T629" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="U629" s="6"/>
+      <c r="U629" s="6" t="s">
+        <v>1663</v>
+      </c>
       <c r="V629" s="6" t="s">
         <v>27</v>
       </c>

</xml_diff>